<commit_message>
Finished Top, Bottom, Left and Right Faces for Model and added Lists to JModel Script
Signed-off-by: HydenJohnson75 <78604065+ToxicOddesey@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ImagesAndExcel/Initial.xlsx
+++ b/ImagesAndExcel/Initial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00220182\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITTralee Files YEAR 3\Computer Graphics\Repos\CompGraphics\ImagesAndExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD76FF66-78E6-441F-AFD2-8546E9C10093}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B4FA69-DA43-4863-A4B1-0AEB6D6AAD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="198" xr2:uid="{ABD2A125-B995-4AC2-8AD9-D0364DF9EFB9}"/>
+    <workbookView xWindow="4500" yWindow="3030" windowWidth="28800" windowHeight="15435" tabRatio="198" xr2:uid="{ABD2A125-B995-4AC2-8AD9-D0364DF9EFB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>X</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>Back</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Bottom</t>
   </si>
 </sst>
 </file>
@@ -443,19 +455,6 @@
       </diagonal>
     </border>
     <border>
-      <left style="dashDot">
-        <color indexed="64"/>
-      </left>
-      <right style="dashDot">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -529,6 +528,21 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="dashDot">
+        <color indexed="64"/>
+      </right>
+      <top style="dashDot">
+        <color indexed="64"/>
+      </top>
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
@@ -629,7 +643,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -637,6 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -951,16 +965,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D07B3A8-AA14-4C79-8BB4-53DEDE84F158}">
-  <dimension ref="B1:AE34"/>
+  <dimension ref="B1:AE55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC17" sqref="AC17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC27" sqref="AC27:AC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="20" max="25" width="5.140625" customWidth="1"/>
     <col min="26" max="26" width="7.140625" customWidth="1"/>
+    <col min="27" max="27" width="2.85546875" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1025,11 +1041,11 @@
       </c>
     </row>
     <row r="5" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="T5" s="11">
         <v>2</v>
       </c>
@@ -1053,13 +1069,13 @@
       </c>
     </row>
     <row r="6" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="42"/>
+      <c r="D6" s="41"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="40"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="39"/>
       <c r="T6" s="11">
         <v>3</v>
       </c>
@@ -1084,17 +1100,17 @@
     </row>
     <row r="7" spans="2:31" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="36"/>
-      <c r="D7" s="41"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="45"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="49"/>
+      <c r="J7" s="44"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="48"/>
       <c r="T7" s="11">
         <v>4</v>
       </c>
@@ -1121,7 +1137,7 @@
       <c r="E8" s="33"/>
       <c r="F8" s="8"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="43"/>
+      <c r="H8" s="42"/>
       <c r="M8" s="8"/>
       <c r="N8" s="4"/>
       <c r="T8" s="11">
@@ -1150,7 +1166,7 @@
       <c r="E9" s="36"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="44"/>
+      <c r="H9" s="43"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="T9" s="11">
@@ -1178,10 +1194,10 @@
     <row r="10" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="32"/>
       <c r="C10" s="31"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="44"/>
+      <c r="H10" s="43"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="T10" s="11">
@@ -1210,10 +1226,10 @@
       <c r="B11" s="31"/>
       <c r="C11" s="5"/>
       <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
+      <c r="E11" s="51"/>
       <c r="F11" s="5"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="45"/>
+      <c r="H11" s="44"/>
       <c r="M11" s="4"/>
       <c r="O11" s="6"/>
       <c r="P11" s="3"/>
@@ -1299,7 +1315,7 @@
       <c r="AB13" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="AC13" s="51">
+      <c r="AC13" s="50">
         <v>30</v>
       </c>
       <c r="AD13" s="13">
@@ -1529,6 +1545,18 @@
       <c r="W23" s="25">
         <v>-1</v>
       </c>
+      <c r="AB23" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC23" s="13">
+        <v>9</v>
+      </c>
+      <c r="AD23" s="13">
+        <v>25</v>
+      </c>
+      <c r="AE23" s="13">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T24" s="11">
@@ -1543,6 +1571,15 @@
       <c r="W24" s="25">
         <v>-1</v>
       </c>
+      <c r="AC24" s="13">
+        <v>9</v>
+      </c>
+      <c r="AD24" s="13">
+        <v>26</v>
+      </c>
+      <c r="AE24" s="13">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T25" s="11">
@@ -1557,6 +1594,15 @@
       <c r="W25" s="25">
         <v>-1</v>
       </c>
+      <c r="AC25" s="13">
+        <v>11</v>
+      </c>
+      <c r="AD25" s="13">
+        <v>27</v>
+      </c>
+      <c r="AE25" s="13">
+        <v>28</v>
+      </c>
     </row>
     <row r="26" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T26" s="11">
@@ -1571,6 +1617,15 @@
       <c r="W26" s="25">
         <v>-1</v>
       </c>
+      <c r="AC26" s="13">
+        <v>11</v>
+      </c>
+      <c r="AD26" s="13">
+        <v>28</v>
+      </c>
+      <c r="AE26" s="13">
+        <v>12</v>
+      </c>
     </row>
     <row r="27" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T27" s="11">
@@ -1585,6 +1640,18 @@
       <c r="W27" s="25">
         <v>-1</v>
       </c>
+      <c r="AB27" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC27" s="13">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="13">
+        <v>25</v>
+      </c>
+      <c r="AE27" s="13">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T28" s="11">
@@ -1599,6 +1666,15 @@
       <c r="W28" s="25">
         <v>-1</v>
       </c>
+      <c r="AC28" s="13">
+        <v>16</v>
+      </c>
+      <c r="AD28" s="13">
+        <v>15</v>
+      </c>
+      <c r="AE28" s="13">
+        <v>31</v>
+      </c>
     </row>
     <row r="29" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T29" s="11">
@@ -1613,6 +1689,15 @@
       <c r="W29" s="25">
         <v>-1</v>
       </c>
+      <c r="AC29" s="13">
+        <v>13</v>
+      </c>
+      <c r="AD29" s="13">
+        <v>30</v>
+      </c>
+      <c r="AE29" s="13">
+        <v>14</v>
+      </c>
     </row>
     <row r="30" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T30" s="11">
@@ -1627,6 +1712,15 @@
       <c r="W30" s="25">
         <v>-1</v>
       </c>
+      <c r="AC30" s="13">
+        <v>13</v>
+      </c>
+      <c r="AD30" s="13">
+        <v>29</v>
+      </c>
+      <c r="AE30" s="13">
+        <v>30</v>
+      </c>
     </row>
     <row r="31" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T31" s="11">
@@ -1641,6 +1735,18 @@
       <c r="W31" s="25">
         <v>-1</v>
       </c>
+      <c r="AB31" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC31" s="13">
+        <v>13</v>
+      </c>
+      <c r="AD31" s="13">
+        <v>12</v>
+      </c>
+      <c r="AE31" s="13">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T32" s="11">
@@ -1655,8 +1761,17 @@
       <c r="W32" s="25">
         <v>-1</v>
       </c>
-    </row>
-    <row r="33" spans="20:23" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC32" s="13">
+        <v>13</v>
+      </c>
+      <c r="AD32" s="13">
+        <v>28</v>
+      </c>
+      <c r="AE32" s="13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T33" s="11">
         <v>30</v>
       </c>
@@ -1669,8 +1784,17 @@
       <c r="W33" s="25">
         <v>-1</v>
       </c>
-    </row>
-    <row r="34" spans="20:23" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC33" s="13">
+        <v>4</v>
+      </c>
+      <c r="AD33" s="13">
+        <v>3</v>
+      </c>
+      <c r="AE33" s="13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T34" s="12">
         <v>31</v>
       </c>
@@ -1683,6 +1807,219 @@
       <c r="W34" s="22">
         <v>-1</v>
       </c>
+      <c r="AC34" s="13">
+        <v>4</v>
+      </c>
+      <c r="AD34" s="13">
+        <v>19</v>
+      </c>
+      <c r="AE34" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC35" s="13">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="13">
+        <v>17</v>
+      </c>
+      <c r="AE35" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC36" s="13">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="13">
+        <v>16</v>
+      </c>
+      <c r="AE36" s="13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC37" s="13">
+        <v>1</v>
+      </c>
+      <c r="AD37" s="13">
+        <v>17</v>
+      </c>
+      <c r="AE37" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC38" s="13">
+        <v>2</v>
+      </c>
+      <c r="AD38" s="13">
+        <v>17</v>
+      </c>
+      <c r="AE38" s="13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC39" s="13">
+        <v>2</v>
+      </c>
+      <c r="AD39" s="13">
+        <v>18</v>
+      </c>
+      <c r="AE39" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC40" s="13">
+        <v>3</v>
+      </c>
+      <c r="AD40" s="13">
+        <v>18</v>
+      </c>
+      <c r="AE40" s="13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB41" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC41" s="13">
+        <v>15</v>
+      </c>
+      <c r="AD41" s="13">
+        <v>30</v>
+      </c>
+      <c r="AE41" s="13">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC42" s="13">
+        <v>15</v>
+      </c>
+      <c r="AD42" s="13">
+        <v>14</v>
+      </c>
+      <c r="AE42" s="13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC43" s="13">
+        <v>11</v>
+      </c>
+      <c r="AD43" s="13">
+        <v>26</v>
+      </c>
+      <c r="AE43" s="13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC44" s="13">
+        <v>11</v>
+      </c>
+      <c r="AD44" s="13">
+        <v>10</v>
+      </c>
+      <c r="AE44" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC45" s="13">
+        <v>4</v>
+      </c>
+      <c r="AD45" s="13">
+        <v>20</v>
+      </c>
+      <c r="AE45" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC46" s="13">
+        <v>20</v>
+      </c>
+      <c r="AD46" s="13">
+        <v>21</v>
+      </c>
+      <c r="AE46" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC47" s="13">
+        <v>5</v>
+      </c>
+      <c r="AD47" s="13">
+        <v>21</v>
+      </c>
+      <c r="AE47" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC48" s="13">
+        <v>21</v>
+      </c>
+      <c r="AD48" s="13">
+        <v>8</v>
+      </c>
+      <c r="AE48" s="13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC49" s="13">
+        <v>8</v>
+      </c>
+      <c r="AD49" s="13">
+        <v>25</v>
+      </c>
+      <c r="AE49" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC50" s="13">
+        <v>8</v>
+      </c>
+      <c r="AD50" s="13">
+        <v>24</v>
+      </c>
+      <c r="AE50" s="13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC51" s="13"/>
+      <c r="AD51" s="13"/>
+      <c r="AE51" s="13"/>
+    </row>
+    <row r="52" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC52" s="13"/>
+      <c r="AD52" s="13"/>
+      <c r="AE52" s="13"/>
+    </row>
+    <row r="53" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC53" s="13"/>
+      <c r="AD53" s="13"/>
+      <c r="AE53" s="13"/>
+    </row>
+    <row r="54" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC54" s="13"/>
+      <c r="AD54" s="13"/>
+      <c r="AE54" s="13"/>
+    </row>
+    <row r="55" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC55" s="13"/>
+      <c r="AD55" s="13"/>
+      <c r="AE55" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created texture map with coordinates based off of 1024x1024
Signed-off-by: HydenJohnson75 <78604065+ToxicOddesey@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ImagesAndExcel/Initial.xlsx
+++ b/ImagesAndExcel/Initial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00220182\Desktop\CompGraphics\ImagesAndExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITTralee Files YEAR 3\Computer Graphics\Repos\CompGraphics\ImagesAndExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E248C5-9502-4A9A-BBF4-E739989209EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CB7C48-E114-4966-A7A8-D7B7B0A7E0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="11400" windowWidth="28800" windowHeight="15435" tabRatio="198" xr2:uid="{ABD2A125-B995-4AC2-8AD9-D0364DF9EFB9}"/>
+    <workbookView xWindow="120" yWindow="5565" windowWidth="28800" windowHeight="15435" tabRatio="198" xr2:uid="{ABD2A125-B995-4AC2-8AD9-D0364DF9EFB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>X</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Bottom</t>
+  </si>
+  <si>
+    <t>Texture Coord</t>
   </si>
 </sst>
 </file>
@@ -552,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -651,6 +654,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D07B3A8-AA14-4C79-8BB4-53DEDE84F158}">
-  <dimension ref="B1:AE55"/>
+  <dimension ref="B1:AM55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AK22" sqref="AK22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -979,8 +991,8 @@
     <col min="28" max="28" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U2" s="14" t="s">
         <v>0</v>
       </c>
@@ -991,7 +1003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T3" s="10">
         <v>0</v>
       </c>
@@ -1016,8 +1028,15 @@
       <c r="AE3" s="13">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AI3" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ3" s="54"/>
+      <c r="AK3" s="54"/>
+      <c r="AL3" s="13"/>
+      <c r="AM3" s="13"/>
+    </row>
+    <row r="4" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T4" s="11">
         <v>1</v>
       </c>
@@ -1039,8 +1058,22 @@
       <c r="AE4" s="13">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ4" s="13">
+        <v>576</v>
+      </c>
+      <c r="AK4" s="13">
+        <v>512</v>
+      </c>
+      <c r="AL4" s="13"/>
+      <c r="AM4" s="13"/>
+    </row>
+    <row r="5" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="39"/>
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
@@ -1067,8 +1100,19 @@
       <c r="AE5" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH5" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="13">
+        <v>544</v>
+      </c>
+      <c r="AK5" s="13">
+        <v>544</v>
+      </c>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="13"/>
+    </row>
+    <row r="6" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="41"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1097,8 +1141,19 @@
       <c r="AE6" s="13">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="2:31" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH6" s="13">
+        <v>2</v>
+      </c>
+      <c r="AJ6" s="13">
+        <v>543</v>
+      </c>
+      <c r="AK6" s="13">
+        <v>575</v>
+      </c>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+    </row>
+    <row r="7" spans="2:39" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="36"/>
       <c r="D7" s="40"/>
       <c r="E7" s="1"/>
@@ -1132,8 +1187,19 @@
       <c r="AE7" s="13">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:31" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH7" s="13">
+        <v>3</v>
+      </c>
+      <c r="AJ7" s="13">
+        <v>576</v>
+      </c>
+      <c r="AK7" s="13">
+        <v>608</v>
+      </c>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+    </row>
+    <row r="8" spans="2:39" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="33"/>
       <c r="F8" s="8"/>
       <c r="G8" s="4"/>
@@ -1161,8 +1227,19 @@
       <c r="AE8" s="13">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH8" s="13">
+        <v>4</v>
+      </c>
+      <c r="AJ8" s="13">
+        <v>544</v>
+      </c>
+      <c r="AK8" s="13">
+        <v>640</v>
+      </c>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+    </row>
+    <row r="9" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E9" s="36"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1190,8 +1267,19 @@
       <c r="AE9" s="13">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH9" s="13">
+        <v>5</v>
+      </c>
+      <c r="AJ9" s="13">
+        <v>512</v>
+      </c>
+      <c r="AK9" s="13">
+        <v>608</v>
+      </c>
+      <c r="AL9" s="13"/>
+      <c r="AM9" s="13"/>
+    </row>
+    <row r="10" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="32"/>
       <c r="C10" s="31"/>
       <c r="E10" s="41"/>
@@ -1221,8 +1309,19 @@
       <c r="AE10" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH10" s="13">
+        <v>6</v>
+      </c>
+      <c r="AJ10" s="13">
+        <v>512</v>
+      </c>
+      <c r="AK10" s="13">
+        <v>575</v>
+      </c>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="13"/>
+    </row>
+    <row r="11" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="31"/>
       <c r="C11" s="5"/>
       <c r="D11" s="38"/>
@@ -1256,8 +1355,19 @@
       <c r="AE11" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="2:31" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH11" s="13">
+        <v>7</v>
+      </c>
+      <c r="AJ11" s="13">
+        <v>512</v>
+      </c>
+      <c r="AK11" s="13">
+        <v>544</v>
+      </c>
+      <c r="AL11" s="13"/>
+      <c r="AM11" s="13"/>
+    </row>
+    <row r="12" spans="2:39" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="32"/>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
@@ -1291,8 +1401,19 @@
       <c r="AE12" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="2:31" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH12" s="13">
+        <v>8</v>
+      </c>
+      <c r="AJ12" s="13">
+        <v>512</v>
+      </c>
+      <c r="AK12" s="13">
+        <v>512</v>
+      </c>
+      <c r="AL12" s="13"/>
+      <c r="AM12" s="13"/>
+    </row>
+    <row r="13" spans="2:39" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="31"/>
       <c r="C13" s="37"/>
       <c r="D13" s="34"/>
@@ -1324,8 +1445,19 @@
       <c r="AE13" s="13">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH13" s="13">
+        <v>9</v>
+      </c>
+      <c r="AJ13" s="13">
+        <v>543</v>
+      </c>
+      <c r="AK13" s="13">
+        <v>480</v>
+      </c>
+      <c r="AL13" s="13"/>
+      <c r="AM13" s="13"/>
+    </row>
+    <row r="14" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T14" s="11">
         <v>11</v>
       </c>
@@ -1347,8 +1479,19 @@
       <c r="AE14" s="13">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH14" s="13">
+        <v>10</v>
+      </c>
+      <c r="AJ14" s="13">
+        <v>671</v>
+      </c>
+      <c r="AK14" s="13">
+        <v>480</v>
+      </c>
+      <c r="AL14" s="13"/>
+      <c r="AM14" s="13"/>
+    </row>
+    <row r="15" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T15" s="11">
         <v>12</v>
       </c>
@@ -1370,8 +1513,19 @@
       <c r="AE15" s="13">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="2:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH15" s="13">
+        <v>11</v>
+      </c>
+      <c r="AJ15" s="13">
+        <v>671</v>
+      </c>
+      <c r="AK15" s="13">
+        <v>416</v>
+      </c>
+      <c r="AL15" s="13"/>
+      <c r="AM15" s="13"/>
+    </row>
+    <row r="16" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T16" s="11">
         <v>13</v>
       </c>
@@ -1393,8 +1547,19 @@
       <c r="AE16" s="13">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH16" s="13">
+        <v>12</v>
+      </c>
+      <c r="AJ16" s="13">
+        <v>704</v>
+      </c>
+      <c r="AK16" s="13">
+        <v>416</v>
+      </c>
+      <c r="AL16" s="13"/>
+      <c r="AM16" s="13"/>
+    </row>
+    <row r="17" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T17" s="11">
         <v>14</v>
       </c>
@@ -1416,8 +1581,19 @@
       <c r="AE17" s="13">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH17" s="13">
+        <v>13</v>
+      </c>
+      <c r="AJ17" s="13">
+        <v>704</v>
+      </c>
+      <c r="AK17" s="13">
+        <v>575</v>
+      </c>
+      <c r="AL17" s="13"/>
+      <c r="AM17" s="13"/>
+    </row>
+    <row r="18" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T18" s="11">
         <v>15</v>
       </c>
@@ -1439,8 +1615,19 @@
       <c r="AE18" s="13">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="20:31" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH18" s="13">
+        <v>14</v>
+      </c>
+      <c r="AJ18" s="13">
+        <v>671</v>
+      </c>
+      <c r="AK18" s="13">
+        <v>575</v>
+      </c>
+      <c r="AL18" s="13"/>
+      <c r="AM18" s="13"/>
+    </row>
+    <row r="19" spans="20:39" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T19" s="26">
         <v>16</v>
       </c>
@@ -1462,8 +1649,19 @@
       <c r="AE19" s="13">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH19" s="13">
+        <v>15</v>
+      </c>
+      <c r="AJ19" s="13">
+        <v>671</v>
+      </c>
+      <c r="AK19" s="13">
+        <v>512</v>
+      </c>
+      <c r="AL19" s="13"/>
+      <c r="AM19" s="13"/>
+    </row>
+    <row r="20" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T20" s="11">
         <v>17</v>
       </c>
@@ -1485,8 +1683,22 @@
       <c r="AE20" s="13">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH20" s="13">
+        <v>16</v>
+      </c>
+      <c r="AI20" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ20" s="13">
+        <v>384</v>
+      </c>
+      <c r="AK20" s="13">
+        <v>512</v>
+      </c>
+      <c r="AL20" s="13"/>
+      <c r="AM20" s="13"/>
+    </row>
+    <row r="21" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T21" s="11">
         <v>18</v>
       </c>
@@ -1508,8 +1720,19 @@
       <c r="AE21" s="13">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH21" s="13">
+        <v>17</v>
+      </c>
+      <c r="AJ21" s="13">
+        <v>416</v>
+      </c>
+      <c r="AK21" s="13">
+        <v>544</v>
+      </c>
+      <c r="AL21" s="13"/>
+      <c r="AM21" s="13"/>
+    </row>
+    <row r="22" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T22" s="11">
         <v>19</v>
       </c>
@@ -1531,8 +1754,19 @@
       <c r="AE22" s="13">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH22" s="13">
+        <v>18</v>
+      </c>
+      <c r="AJ22" s="13">
+        <v>416</v>
+      </c>
+      <c r="AK22" s="13">
+        <v>575</v>
+      </c>
+      <c r="AL22" s="13"/>
+      <c r="AM22" s="13"/>
+    </row>
+    <row r="23" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T23" s="11">
         <v>20</v>
       </c>
@@ -1557,8 +1791,19 @@
       <c r="AE23" s="13">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH23" s="13">
+        <v>19</v>
+      </c>
+      <c r="AJ23" s="13">
+        <v>384</v>
+      </c>
+      <c r="AK23" s="13">
+        <v>608</v>
+      </c>
+      <c r="AL23" s="13"/>
+      <c r="AM23" s="13"/>
+    </row>
+    <row r="24" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T24" s="11">
         <v>21</v>
       </c>
@@ -1580,8 +1825,19 @@
       <c r="AE24" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH24" s="13">
+        <v>20</v>
+      </c>
+      <c r="AJ24" s="13">
+        <v>416</v>
+      </c>
+      <c r="AK24" s="13">
+        <v>640</v>
+      </c>
+      <c r="AL24" s="13"/>
+      <c r="AM24" s="13"/>
+    </row>
+    <row r="25" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T25" s="11">
         <v>22</v>
       </c>
@@ -1603,8 +1859,19 @@
       <c r="AE25" s="13">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH25" s="13">
+        <v>21</v>
+      </c>
+      <c r="AJ25" s="13">
+        <v>448</v>
+      </c>
+      <c r="AK25" s="13">
+        <v>608</v>
+      </c>
+      <c r="AL25" s="13"/>
+      <c r="AM25" s="13"/>
+    </row>
+    <row r="26" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T26" s="11">
         <v>23</v>
       </c>
@@ -1626,8 +1893,19 @@
       <c r="AE26" s="13">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH26" s="13">
+        <v>22</v>
+      </c>
+      <c r="AJ26" s="13">
+        <v>448</v>
+      </c>
+      <c r="AK26" s="13">
+        <v>575</v>
+      </c>
+      <c r="AL26" s="13"/>
+      <c r="AM26" s="13"/>
+    </row>
+    <row r="27" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T27" s="11">
         <v>24</v>
       </c>
@@ -1652,8 +1930,19 @@
       <c r="AE27" s="13">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH27" s="13">
+        <v>23</v>
+      </c>
+      <c r="AJ27" s="13">
+        <v>448</v>
+      </c>
+      <c r="AK27" s="13">
+        <v>544</v>
+      </c>
+      <c r="AL27" s="13"/>
+      <c r="AM27" s="13"/>
+    </row>
+    <row r="28" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T28" s="11">
         <v>25</v>
       </c>
@@ -1675,8 +1964,19 @@
       <c r="AE28" s="13">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH28" s="13">
+        <v>24</v>
+      </c>
+      <c r="AJ28" s="13">
+        <v>228</v>
+      </c>
+      <c r="AK28" s="13">
+        <v>512</v>
+      </c>
+      <c r="AL28" s="13"/>
+      <c r="AM28" s="13"/>
+    </row>
+    <row r="29" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T29" s="11">
         <v>26</v>
       </c>
@@ -1698,8 +1998,19 @@
       <c r="AE29" s="13">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH29" s="13">
+        <v>25</v>
+      </c>
+      <c r="AJ29" s="13">
+        <v>416</v>
+      </c>
+      <c r="AK29" s="13">
+        <v>480</v>
+      </c>
+      <c r="AL29" s="13"/>
+      <c r="AM29" s="13"/>
+    </row>
+    <row r="30" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T30" s="11">
         <v>27</v>
       </c>
@@ -1721,8 +2032,19 @@
       <c r="AE30" s="13">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH30" s="13">
+        <v>26</v>
+      </c>
+      <c r="AJ30" s="13">
+        <v>288</v>
+      </c>
+      <c r="AK30" s="13">
+        <v>480</v>
+      </c>
+      <c r="AL30" s="13"/>
+      <c r="AM30" s="13"/>
+    </row>
+    <row r="31" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T31" s="11">
         <v>28</v>
       </c>
@@ -1747,8 +2069,19 @@
       <c r="AE31" s="13">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH31" s="13">
+        <v>27</v>
+      </c>
+      <c r="AJ31" s="13">
+        <v>288</v>
+      </c>
+      <c r="AK31" s="13">
+        <v>416</v>
+      </c>
+      <c r="AL31" s="13"/>
+      <c r="AM31" s="13"/>
+    </row>
+    <row r="32" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T32" s="11">
         <v>29</v>
       </c>
@@ -1770,8 +2103,19 @@
       <c r="AE32" s="13">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH32" s="13">
+        <v>28</v>
+      </c>
+      <c r="AJ32" s="13">
+        <v>255</v>
+      </c>
+      <c r="AK32" s="13">
+        <v>416</v>
+      </c>
+      <c r="AL32" s="13"/>
+      <c r="AM32" s="13"/>
+    </row>
+    <row r="33" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T33" s="11">
         <v>30</v>
       </c>
@@ -1793,8 +2137,19 @@
       <c r="AE33" s="13">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="20:31" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH33" s="13">
+        <v>29</v>
+      </c>
+      <c r="AJ33" s="13">
+        <v>255</v>
+      </c>
+      <c r="AK33" s="13">
+        <v>575</v>
+      </c>
+      <c r="AL33" s="13"/>
+      <c r="AM33" s="13"/>
+    </row>
+    <row r="34" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T34" s="12">
         <v>31</v>
       </c>
@@ -1816,8 +2171,19 @@
       <c r="AE34" s="13">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH34" s="13">
+        <v>30</v>
+      </c>
+      <c r="AJ34" s="13">
+        <v>288</v>
+      </c>
+      <c r="AK34" s="13">
+        <v>575</v>
+      </c>
+      <c r="AL34" s="13"/>
+      <c r="AM34" s="13"/>
+    </row>
+    <row r="35" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC35" s="13">
         <v>0</v>
       </c>
@@ -1827,8 +2193,19 @@
       <c r="AE35" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH35" s="13">
+        <v>31</v>
+      </c>
+      <c r="AJ35" s="13">
+        <v>288</v>
+      </c>
+      <c r="AK35" s="13">
+        <v>512</v>
+      </c>
+      <c r="AL35" s="13"/>
+      <c r="AM35" s="13"/>
+    </row>
+    <row r="36" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC36" s="13">
         <v>0</v>
       </c>
@@ -1838,8 +2215,12 @@
       <c r="AE36" s="13">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ36" s="13"/>
+      <c r="AK36" s="13"/>
+      <c r="AL36" s="13"/>
+      <c r="AM36" s="13"/>
+    </row>
+    <row r="37" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC37" s="13">
         <v>1</v>
       </c>
@@ -1849,8 +2230,12 @@
       <c r="AE37" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ37" s="13"/>
+      <c r="AK37" s="13"/>
+      <c r="AL37" s="13"/>
+      <c r="AM37" s="13"/>
+    </row>
+    <row r="38" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC38" s="13">
         <v>2</v>
       </c>
@@ -1860,8 +2245,12 @@
       <c r="AE38" s="13">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ38" s="13"/>
+      <c r="AK38" s="13"/>
+      <c r="AL38" s="13"/>
+      <c r="AM38" s="13"/>
+    </row>
+    <row r="39" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC39" s="13">
         <v>2</v>
       </c>
@@ -1871,8 +2260,12 @@
       <c r="AE39" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ39" s="13"/>
+      <c r="AK39" s="13"/>
+      <c r="AL39" s="13"/>
+      <c r="AM39" s="13"/>
+    </row>
+    <row r="40" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC40" s="13">
         <v>3</v>
       </c>
@@ -1882,8 +2275,12 @@
       <c r="AE40" s="13">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ40" s="13"/>
+      <c r="AK40" s="13"/>
+      <c r="AL40" s="13"/>
+      <c r="AM40" s="13"/>
+    </row>
+    <row r="41" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AB41" s="30" t="s">
         <v>8</v>
       </c>
@@ -1896,8 +2293,12 @@
       <c r="AE41" s="13">
         <v>31</v>
       </c>
-    </row>
-    <row r="42" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ41" s="13"/>
+      <c r="AK41" s="13"/>
+      <c r="AL41" s="13"/>
+      <c r="AM41" s="13"/>
+    </row>
+    <row r="42" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC42" s="13">
         <v>15</v>
       </c>
@@ -1907,8 +2308,12 @@
       <c r="AE42" s="13">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ42" s="13"/>
+      <c r="AK42" s="13"/>
+      <c r="AL42" s="13"/>
+      <c r="AM42" s="13"/>
+    </row>
+    <row r="43" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC43" s="13">
         <v>11</v>
       </c>
@@ -1918,8 +2323,12 @@
       <c r="AE43" s="13">
         <v>27</v>
       </c>
-    </row>
-    <row r="44" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ43" s="13"/>
+      <c r="AK43" s="13"/>
+      <c r="AL43" s="13"/>
+      <c r="AM43" s="13"/>
+    </row>
+    <row r="44" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC44" s="13">
         <v>11</v>
       </c>
@@ -1929,8 +2338,12 @@
       <c r="AE44" s="13">
         <v>26</v>
       </c>
-    </row>
-    <row r="45" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ44" s="13"/>
+      <c r="AK44" s="13"/>
+      <c r="AL44" s="13"/>
+      <c r="AM44" s="13"/>
+    </row>
+    <row r="45" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC45" s="13">
         <v>4</v>
       </c>
@@ -1940,8 +2353,12 @@
       <c r="AE45" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ45" s="13"/>
+      <c r="AK45" s="13"/>
+      <c r="AL45" s="13"/>
+      <c r="AM45" s="13"/>
+    </row>
+    <row r="46" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC46" s="13">
         <v>20</v>
       </c>
@@ -1951,8 +2368,12 @@
       <c r="AE46" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ46" s="13"/>
+      <c r="AK46" s="13"/>
+      <c r="AL46" s="13"/>
+      <c r="AM46" s="13"/>
+    </row>
+    <row r="47" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC47" s="13">
         <v>5</v>
       </c>
@@ -1962,8 +2383,12 @@
       <c r="AE47" s="13">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="20:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ47" s="13"/>
+      <c r="AK47" s="13"/>
+      <c r="AL47" s="13"/>
+      <c r="AM47" s="13"/>
+    </row>
+    <row r="48" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC48" s="13">
         <v>21</v>
       </c>
@@ -1973,8 +2398,12 @@
       <c r="AE48" s="13">
         <v>24</v>
       </c>
-    </row>
-    <row r="49" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ48" s="13"/>
+      <c r="AK48" s="13"/>
+      <c r="AL48" s="13"/>
+      <c r="AM48" s="13"/>
+    </row>
+    <row r="49" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC49" s="13">
         <v>8</v>
       </c>
@@ -1984,8 +2413,12 @@
       <c r="AE49" s="13">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ49" s="13"/>
+      <c r="AK49" s="13"/>
+      <c r="AL49" s="13"/>
+      <c r="AM49" s="13"/>
+    </row>
+    <row r="50" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC50" s="13">
         <v>8</v>
       </c>
@@ -1995,28 +2428,32 @@
       <c r="AE50" s="13">
         <v>25</v>
       </c>
-    </row>
-    <row r="51" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ50" s="13"/>
+      <c r="AK50" s="13"/>
+      <c r="AL50" s="13"/>
+      <c r="AM50" s="13"/>
+    </row>
+    <row r="51" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC51" s="13"/>
       <c r="AD51" s="13"/>
       <c r="AE51" s="13"/>
     </row>
-    <row r="52" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC52" s="13"/>
       <c r="AD52" s="13"/>
       <c r="AE52" s="13"/>
     </row>
-    <row r="53" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC53" s="13"/>
       <c r="AD53" s="13"/>
       <c r="AE53" s="13"/>
     </row>
-    <row r="54" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC54" s="13"/>
       <c r="AD54" s="13"/>
       <c r="AE54" s="13"/>
     </row>
-    <row r="55" spans="29:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC55" s="13"/>
       <c r="AD55" s="13"/>
       <c r="AE55" s="13"/>

</xml_diff>

<commit_message>
Added Texture coords and index
Signed-off-by: HydenJohnson75 <78604065+ToxicOddesey@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ImagesAndExcel/Initial.xlsx
+++ b/ImagesAndExcel/Initial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITTralee Files YEAR 3\Computer Graphics\Repos\CompGraphics\ImagesAndExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CB7C48-E114-4966-A7A8-D7B7B0A7E0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7893F46A-1EB3-4DA6-B687-1608E3543125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="5565" windowWidth="28800" windowHeight="15435" tabRatio="198" xr2:uid="{ABD2A125-B995-4AC2-8AD9-D0364DF9EFB9}"/>
+    <workbookView xWindow="4320" yWindow="3435" windowWidth="28800" windowHeight="15435" tabRatio="198" xr2:uid="{ABD2A125-B995-4AC2-8AD9-D0364DF9EFB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -977,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D07B3A8-AA14-4C79-8BB4-53DEDE84F158}">
-  <dimension ref="B1:AM55"/>
+  <dimension ref="B1:AT55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AK22" sqref="AK22"/>
+    <sheetView tabSelected="1" topLeftCell="O7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3:U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -991,8 +991,8 @@
     <col min="28" max="28" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U2" s="14" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T3" s="10">
         <v>0</v>
       </c>
@@ -1036,7 +1036,7 @@
       <c r="AL3" s="13"/>
       <c r="AM3" s="13"/>
     </row>
-    <row r="4" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T4" s="11">
         <v>1</v>
       </c>
@@ -1072,8 +1072,14 @@
       </c>
       <c r="AL4" s="13"/>
       <c r="AM4" s="13"/>
-    </row>
-    <row r="5" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO4">
+        <v>0.5625</v>
+      </c>
+      <c r="AP4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="39"/>
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
@@ -1111,8 +1117,14 @@
       </c>
       <c r="AL5" s="13"/>
       <c r="AM5" s="13"/>
-    </row>
-    <row r="6" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO5">
+        <v>0.53125</v>
+      </c>
+      <c r="AP5">
+        <v>0.53125</v>
+      </c>
+    </row>
+    <row r="6" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="41"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1152,8 +1164,14 @@
       </c>
       <c r="AL6" s="13"/>
       <c r="AM6" s="13"/>
-    </row>
-    <row r="7" spans="2:39" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO6">
+        <v>0.5302734375</v>
+      </c>
+      <c r="AP6">
+        <v>0.5615234375</v>
+      </c>
+    </row>
+    <row r="7" spans="2:42" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="36"/>
       <c r="D7" s="40"/>
       <c r="E7" s="1"/>
@@ -1198,8 +1216,14 @@
       </c>
       <c r="AL7" s="13"/>
       <c r="AM7" s="13"/>
-    </row>
-    <row r="8" spans="2:39" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO7">
+        <v>0.5625</v>
+      </c>
+      <c r="AP7">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="8" spans="2:42" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="33"/>
       <c r="F8" s="8"/>
       <c r="G8" s="4"/>
@@ -1238,8 +1262,14 @@
       </c>
       <c r="AL8" s="13"/>
       <c r="AM8" s="13"/>
-    </row>
-    <row r="9" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO8">
+        <v>0.53125</v>
+      </c>
+      <c r="AP8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="9" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E9" s="36"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1278,8 +1308,14 @@
       </c>
       <c r="AL9" s="13"/>
       <c r="AM9" s="13"/>
-    </row>
-    <row r="10" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO9">
+        <v>0.5</v>
+      </c>
+      <c r="AP9">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="10" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="32"/>
       <c r="C10" s="31"/>
       <c r="E10" s="41"/>
@@ -1320,8 +1356,14 @@
       </c>
       <c r="AL10" s="13"/>
       <c r="AM10" s="13"/>
-    </row>
-    <row r="11" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO10">
+        <v>0.5</v>
+      </c>
+      <c r="AP10">
+        <v>0.5615234375</v>
+      </c>
+    </row>
+    <row r="11" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="31"/>
       <c r="C11" s="5"/>
       <c r="D11" s="38"/>
@@ -1366,8 +1408,14 @@
       </c>
       <c r="AL11" s="13"/>
       <c r="AM11" s="13"/>
-    </row>
-    <row r="12" spans="2:39" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO11">
+        <v>0.5</v>
+      </c>
+      <c r="AP11">
+        <v>0.53125</v>
+      </c>
+    </row>
+    <row r="12" spans="2:42" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="32"/>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
@@ -1412,8 +1460,14 @@
       </c>
       <c r="AL12" s="13"/>
       <c r="AM12" s="13"/>
-    </row>
-    <row r="13" spans="2:39" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO12">
+        <v>0.5</v>
+      </c>
+      <c r="AP12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:42" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="31"/>
       <c r="C13" s="37"/>
       <c r="D13" s="34"/>
@@ -1456,8 +1510,14 @@
       </c>
       <c r="AL13" s="13"/>
       <c r="AM13" s="13"/>
-    </row>
-    <row r="14" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO13">
+        <v>0.5302734375</v>
+      </c>
+      <c r="AP13">
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="14" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T14" s="11">
         <v>11</v>
       </c>
@@ -1490,8 +1550,14 @@
       </c>
       <c r="AL14" s="13"/>
       <c r="AM14" s="13"/>
-    </row>
-    <row r="15" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO14">
+        <v>0.6552734375</v>
+      </c>
+      <c r="AP14">
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="15" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T15" s="11">
         <v>12</v>
       </c>
@@ -1524,8 +1590,14 @@
       </c>
       <c r="AL15" s="13"/>
       <c r="AM15" s="13"/>
-    </row>
-    <row r="16" spans="2:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO15">
+        <v>0.6552734375</v>
+      </c>
+      <c r="AP15">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="16" spans="2:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T16" s="11">
         <v>13</v>
       </c>
@@ -1558,8 +1630,14 @@
       </c>
       <c r="AL16" s="13"/>
       <c r="AM16" s="13"/>
-    </row>
-    <row r="17" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO16">
+        <v>0.6875</v>
+      </c>
+      <c r="AP16">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="17" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T17" s="11">
         <v>14</v>
       </c>
@@ -1592,8 +1670,14 @@
       </c>
       <c r="AL17" s="13"/>
       <c r="AM17" s="13"/>
-    </row>
-    <row r="18" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO17">
+        <v>0.6875</v>
+      </c>
+      <c r="AP17">
+        <v>0.5615234375</v>
+      </c>
+    </row>
+    <row r="18" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T18" s="11">
         <v>15</v>
       </c>
@@ -1626,8 +1710,14 @@
       </c>
       <c r="AL18" s="13"/>
       <c r="AM18" s="13"/>
-    </row>
-    <row r="19" spans="20:39" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO18">
+        <v>0.6552734375</v>
+      </c>
+      <c r="AP18">
+        <v>0.5615234375</v>
+      </c>
+    </row>
+    <row r="19" spans="20:46" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T19" s="26">
         <v>16</v>
       </c>
@@ -1660,8 +1750,14 @@
       </c>
       <c r="AL19" s="13"/>
       <c r="AM19" s="13"/>
-    </row>
-    <row r="20" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO19">
+        <v>0.6552734375</v>
+      </c>
+      <c r="AP19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T20" s="11">
         <v>17</v>
       </c>
@@ -1697,8 +1793,14 @@
       </c>
       <c r="AL20" s="13"/>
       <c r="AM20" s="13"/>
-    </row>
-    <row r="21" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO20">
+        <v>0.375</v>
+      </c>
+      <c r="AP20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T21" s="11">
         <v>18</v>
       </c>
@@ -1731,8 +1833,17 @@
       </c>
       <c r="AL21" s="13"/>
       <c r="AM21" s="13"/>
-    </row>
-    <row r="22" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO21">
+        <v>0.40625</v>
+      </c>
+      <c r="AP21">
+        <v>0.53125</v>
+      </c>
+      <c r="AT21">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="22" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T22" s="11">
         <v>19</v>
       </c>
@@ -1765,8 +1876,14 @@
       </c>
       <c r="AL22" s="13"/>
       <c r="AM22" s="13"/>
-    </row>
-    <row r="23" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO22">
+        <v>0.40625</v>
+      </c>
+      <c r="AP22">
+        <v>0.5615234375</v>
+      </c>
+    </row>
+    <row r="23" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T23" s="11">
         <v>20</v>
       </c>
@@ -1802,8 +1919,14 @@
       </c>
       <c r="AL23" s="13"/>
       <c r="AM23" s="13"/>
-    </row>
-    <row r="24" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO23">
+        <v>0.375</v>
+      </c>
+      <c r="AP23">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="24" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T24" s="11">
         <v>21</v>
       </c>
@@ -1836,8 +1959,14 @@
       </c>
       <c r="AL24" s="13"/>
       <c r="AM24" s="13"/>
-    </row>
-    <row r="25" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO24">
+        <v>0.40625</v>
+      </c>
+      <c r="AP24">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="25" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T25" s="11">
         <v>22</v>
       </c>
@@ -1870,8 +1999,14 @@
       </c>
       <c r="AL25" s="13"/>
       <c r="AM25" s="13"/>
-    </row>
-    <row r="26" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO25">
+        <v>0.4375</v>
+      </c>
+      <c r="AP25">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="26" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T26" s="11">
         <v>23</v>
       </c>
@@ -1904,8 +2039,14 @@
       </c>
       <c r="AL26" s="13"/>
       <c r="AM26" s="13"/>
-    </row>
-    <row r="27" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO26">
+        <v>0.4375</v>
+      </c>
+      <c r="AP26">
+        <v>0.5615234375</v>
+      </c>
+    </row>
+    <row r="27" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T27" s="11">
         <v>24</v>
       </c>
@@ -1941,8 +2082,14 @@
       </c>
       <c r="AL27" s="13"/>
       <c r="AM27" s="13"/>
-    </row>
-    <row r="28" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO27">
+        <v>0.4375</v>
+      </c>
+      <c r="AP27">
+        <v>0.53125</v>
+      </c>
+    </row>
+    <row r="28" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T28" s="11">
         <v>25</v>
       </c>
@@ -1975,8 +2122,14 @@
       </c>
       <c r="AL28" s="13"/>
       <c r="AM28" s="13"/>
-    </row>
-    <row r="29" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO28">
+        <v>0.22265625</v>
+      </c>
+      <c r="AP28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T29" s="11">
         <v>26</v>
       </c>
@@ -2009,8 +2162,14 @@
       </c>
       <c r="AL29" s="13"/>
       <c r="AM29" s="13"/>
-    </row>
-    <row r="30" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO29">
+        <v>0.40625</v>
+      </c>
+      <c r="AP29">
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="30" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T30" s="11">
         <v>27</v>
       </c>
@@ -2043,8 +2202,14 @@
       </c>
       <c r="AL30" s="13"/>
       <c r="AM30" s="13"/>
-    </row>
-    <row r="31" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO30">
+        <v>0.28125</v>
+      </c>
+      <c r="AP30">
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="31" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T31" s="11">
         <v>28</v>
       </c>
@@ -2080,8 +2245,14 @@
       </c>
       <c r="AL31" s="13"/>
       <c r="AM31" s="13"/>
-    </row>
-    <row r="32" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO31">
+        <v>0.28125</v>
+      </c>
+      <c r="AP31">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="32" spans="20:46" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T32" s="11">
         <v>29</v>
       </c>
@@ -2114,8 +2285,14 @@
       </c>
       <c r="AL32" s="13"/>
       <c r="AM32" s="13"/>
-    </row>
-    <row r="33" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO32">
+        <v>0.2490234375</v>
+      </c>
+      <c r="AP32">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="33" spans="20:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T33" s="11">
         <v>30</v>
       </c>
@@ -2148,8 +2325,14 @@
       </c>
       <c r="AL33" s="13"/>
       <c r="AM33" s="13"/>
-    </row>
-    <row r="34" spans="20:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO33">
+        <v>0.2490234375</v>
+      </c>
+      <c r="AP33">
+        <v>0.5615234375</v>
+      </c>
+    </row>
+    <row r="34" spans="20:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T34" s="12">
         <v>31</v>
       </c>
@@ -2182,8 +2365,14 @@
       </c>
       <c r="AL34" s="13"/>
       <c r="AM34" s="13"/>
-    </row>
-    <row r="35" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO34">
+        <v>0.28125</v>
+      </c>
+      <c r="AP34">
+        <v>0.5615234375</v>
+      </c>
+    </row>
+    <row r="35" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC35" s="13">
         <v>0</v>
       </c>
@@ -2204,8 +2393,14 @@
       </c>
       <c r="AL35" s="13"/>
       <c r="AM35" s="13"/>
-    </row>
-    <row r="36" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO35">
+        <v>0.28125</v>
+      </c>
+      <c r="AP35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC36" s="13">
         <v>0</v>
       </c>
@@ -2220,7 +2415,7 @@
       <c r="AL36" s="13"/>
       <c r="AM36" s="13"/>
     </row>
-    <row r="37" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC37" s="13">
         <v>1</v>
       </c>
@@ -2235,7 +2430,7 @@
       <c r="AL37" s="13"/>
       <c r="AM37" s="13"/>
     </row>
-    <row r="38" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC38" s="13">
         <v>2</v>
       </c>
@@ -2250,7 +2445,7 @@
       <c r="AL38" s="13"/>
       <c r="AM38" s="13"/>
     </row>
-    <row r="39" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC39" s="13">
         <v>2</v>
       </c>
@@ -2265,7 +2460,7 @@
       <c r="AL39" s="13"/>
       <c r="AM39" s="13"/>
     </row>
-    <row r="40" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC40" s="13">
         <v>3</v>
       </c>
@@ -2280,7 +2475,7 @@
       <c r="AL40" s="13"/>
       <c r="AM40" s="13"/>
     </row>
-    <row r="41" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AB41" s="30" t="s">
         <v>8</v>
       </c>
@@ -2298,7 +2493,7 @@
       <c r="AL41" s="13"/>
       <c r="AM41" s="13"/>
     </row>
-    <row r="42" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC42" s="13">
         <v>15</v>
       </c>
@@ -2313,7 +2508,7 @@
       <c r="AL42" s="13"/>
       <c r="AM42" s="13"/>
     </row>
-    <row r="43" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC43" s="13">
         <v>11</v>
       </c>
@@ -2328,7 +2523,7 @@
       <c r="AL43" s="13"/>
       <c r="AM43" s="13"/>
     </row>
-    <row r="44" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC44" s="13">
         <v>11</v>
       </c>
@@ -2343,7 +2538,7 @@
       <c r="AL44" s="13"/>
       <c r="AM44" s="13"/>
     </row>
-    <row r="45" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC45" s="13">
         <v>4</v>
       </c>
@@ -2358,7 +2553,7 @@
       <c r="AL45" s="13"/>
       <c r="AM45" s="13"/>
     </row>
-    <row r="46" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC46" s="13">
         <v>20</v>
       </c>
@@ -2373,7 +2568,7 @@
       <c r="AL46" s="13"/>
       <c r="AM46" s="13"/>
     </row>
-    <row r="47" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC47" s="13">
         <v>5</v>
       </c>
@@ -2388,7 +2583,7 @@
       <c r="AL47" s="13"/>
       <c r="AM47" s="13"/>
     </row>
-    <row r="48" spans="20:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC48" s="13">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Added more texture parts
Signed-off-by: HydenJohnson75 <78604065+ToxicOddesey@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ImagesAndExcel/Initial.xlsx
+++ b/ImagesAndExcel/Initial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITTralee Files YEAR 3\Computer Graphics\Repos\CompGraphics\ImagesAndExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7893F46A-1EB3-4DA6-B687-1608E3543125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2298BBE1-8E90-45CF-90B5-B041E7AF307F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="3435" windowWidth="28800" windowHeight="15435" tabRatio="198" xr2:uid="{ABD2A125-B995-4AC2-8AD9-D0364DF9EFB9}"/>
+    <workbookView xWindow="0" yWindow="4095" windowWidth="28800" windowHeight="14190" tabRatio="198" xr2:uid="{ABD2A125-B995-4AC2-8AD9-D0364DF9EFB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -977,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D07B3A8-AA14-4C79-8BB4-53DEDE84F158}">
-  <dimension ref="B1:AT55"/>
+  <dimension ref="B1:AT97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3:U34"/>
+    <sheetView tabSelected="1" topLeftCell="O74" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AP40" sqref="AP40:AQ97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2292,7 +2292,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="33" spans="20:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="20:43" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T33" s="11">
         <v>30</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>0.5615234375</v>
       </c>
     </row>
-    <row r="34" spans="20:42" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="20:43" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T34" s="12">
         <v>31</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>0.5615234375</v>
       </c>
     </row>
-    <row r="35" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC35" s="13">
         <v>0</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC36" s="13">
         <v>0</v>
       </c>
@@ -2415,7 +2415,7 @@
       <c r="AL36" s="13"/>
       <c r="AM36" s="13"/>
     </row>
-    <row r="37" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC37" s="13">
         <v>1</v>
       </c>
@@ -2430,7 +2430,7 @@
       <c r="AL37" s="13"/>
       <c r="AM37" s="13"/>
     </row>
-    <row r="38" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC38" s="13">
         <v>2</v>
       </c>
@@ -2445,7 +2445,7 @@
       <c r="AL38" s="13"/>
       <c r="AM38" s="13"/>
     </row>
-    <row r="39" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC39" s="13">
         <v>2</v>
       </c>
@@ -2460,7 +2460,7 @@
       <c r="AL39" s="13"/>
       <c r="AM39" s="13"/>
     </row>
-    <row r="40" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC40" s="13">
         <v>3</v>
       </c>
@@ -2474,8 +2474,17 @@
       <c r="AK40" s="13"/>
       <c r="AL40" s="13"/>
       <c r="AM40" s="13"/>
-    </row>
-    <row r="41" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN40">
+        <v>0</v>
+      </c>
+      <c r="AP40">
+        <v>511</v>
+      </c>
+      <c r="AQ40">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="41" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AB41" s="30" t="s">
         <v>8</v>
       </c>
@@ -2492,8 +2501,17 @@
       <c r="AK41" s="13"/>
       <c r="AL41" s="13"/>
       <c r="AM41" s="13"/>
-    </row>
-    <row r="42" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN41">
+        <v>1</v>
+      </c>
+      <c r="AP41">
+        <v>447</v>
+      </c>
+      <c r="AQ41">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="42" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC42" s="13">
         <v>15</v>
       </c>
@@ -2507,8 +2525,17 @@
       <c r="AK42" s="13"/>
       <c r="AL42" s="13"/>
       <c r="AM42" s="13"/>
-    </row>
-    <row r="43" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN42">
+        <v>2</v>
+      </c>
+      <c r="AP42">
+        <v>381</v>
+      </c>
+      <c r="AQ42">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="43" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC43" s="13">
         <v>11</v>
       </c>
@@ -2522,8 +2549,17 @@
       <c r="AK43" s="13"/>
       <c r="AL43" s="13"/>
       <c r="AM43" s="13"/>
-    </row>
-    <row r="44" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN43">
+        <v>3</v>
+      </c>
+      <c r="AP43">
+        <v>319</v>
+      </c>
+      <c r="AQ43">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="44" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC44" s="13">
         <v>11</v>
       </c>
@@ -2537,8 +2573,17 @@
       <c r="AK44" s="13"/>
       <c r="AL44" s="13"/>
       <c r="AM44" s="13"/>
-    </row>
-    <row r="45" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN44">
+        <v>4</v>
+      </c>
+      <c r="AP44">
+        <v>256</v>
+      </c>
+      <c r="AQ44">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="45" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC45" s="13">
         <v>4</v>
       </c>
@@ -2552,8 +2597,17 @@
       <c r="AK45" s="13"/>
       <c r="AL45" s="13"/>
       <c r="AM45" s="13"/>
-    </row>
-    <row r="46" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN45">
+        <v>5</v>
+      </c>
+      <c r="AP45">
+        <v>318</v>
+      </c>
+      <c r="AQ45">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="46" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC46" s="13">
         <v>20</v>
       </c>
@@ -2567,8 +2621,17 @@
       <c r="AK46" s="13"/>
       <c r="AL46" s="13"/>
       <c r="AM46" s="13"/>
-    </row>
-    <row r="47" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN46">
+        <v>6</v>
+      </c>
+      <c r="AP46">
+        <v>383</v>
+      </c>
+      <c r="AQ46">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="47" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC47" s="13">
         <v>5</v>
       </c>
@@ -2582,8 +2645,17 @@
       <c r="AK47" s="13"/>
       <c r="AL47" s="13"/>
       <c r="AM47" s="13"/>
-    </row>
-    <row r="48" spans="20:42" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN47">
+        <v>7</v>
+      </c>
+      <c r="AP47">
+        <v>446</v>
+      </c>
+      <c r="AQ47">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="48" spans="20:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC48" s="13">
         <v>21</v>
       </c>
@@ -2597,8 +2669,17 @@
       <c r="AK48" s="13"/>
       <c r="AL48" s="13"/>
       <c r="AM48" s="13"/>
-    </row>
-    <row r="49" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN48">
+        <v>8</v>
+      </c>
+      <c r="AP48">
+        <v>511</v>
+      </c>
+      <c r="AQ48">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="49" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC49" s="13">
         <v>8</v>
       </c>
@@ -2612,8 +2693,17 @@
       <c r="AK49" s="13"/>
       <c r="AL49" s="13"/>
       <c r="AM49" s="13"/>
-    </row>
-    <row r="50" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN49">
+        <v>9</v>
+      </c>
+      <c r="AP49">
+        <v>575</v>
+      </c>
+      <c r="AQ49">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="50" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC50" s="13">
         <v>8</v>
       </c>
@@ -2627,31 +2717,547 @@
       <c r="AK50" s="13"/>
       <c r="AL50" s="13"/>
       <c r="AM50" s="13"/>
-    </row>
-    <row r="51" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN50">
+        <v>10</v>
+      </c>
+      <c r="AP50">
+        <v>576</v>
+      </c>
+      <c r="AQ50">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC51" s="13"/>
       <c r="AD51" s="13"/>
       <c r="AE51" s="13"/>
-    </row>
-    <row r="52" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN51">
+        <v>11</v>
+      </c>
+      <c r="AP51">
+        <v>704</v>
+      </c>
+      <c r="AQ51">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC52" s="13"/>
       <c r="AD52" s="13"/>
       <c r="AE52" s="13"/>
-    </row>
-    <row r="53" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN52">
+        <v>12</v>
+      </c>
+      <c r="AP52">
+        <v>704</v>
+      </c>
+      <c r="AQ52">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC53" s="13"/>
       <c r="AD53" s="13"/>
       <c r="AE53" s="13"/>
-    </row>
-    <row r="54" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN53">
+        <v>13</v>
+      </c>
+      <c r="AP53">
+        <v>383</v>
+      </c>
+      <c r="AQ53">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC54" s="13"/>
       <c r="AD54" s="13"/>
       <c r="AE54" s="13"/>
-    </row>
-    <row r="55" spans="29:39" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN54">
+        <v>14</v>
+      </c>
+      <c r="AP54">
+        <v>383</v>
+      </c>
+      <c r="AQ54">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC55" s="13"/>
       <c r="AD55" s="13"/>
       <c r="AE55" s="13"/>
+      <c r="AN55">
+        <v>15</v>
+      </c>
+      <c r="AP55">
+        <v>511</v>
+      </c>
+      <c r="AQ55">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="56" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN56">
+        <v>16</v>
+      </c>
+      <c r="AP56">
+        <v>512</v>
+      </c>
+      <c r="AQ56">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="57" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN57">
+        <v>17</v>
+      </c>
+      <c r="AP57">
+        <v>447</v>
+      </c>
+      <c r="AQ57">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="58" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN58">
+        <v>18</v>
+      </c>
+      <c r="AP58">
+        <v>383</v>
+      </c>
+      <c r="AQ58">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="59" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN59">
+        <v>19</v>
+      </c>
+      <c r="AP59">
+        <v>318</v>
+      </c>
+      <c r="AQ59">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="60" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN60">
+        <v>20</v>
+      </c>
+      <c r="AP60">
+        <v>256</v>
+      </c>
+      <c r="AQ60">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="61" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN61">
+        <v>21</v>
+      </c>
+      <c r="AP61">
+        <v>319</v>
+      </c>
+      <c r="AQ61">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="62" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN62">
+        <v>22</v>
+      </c>
+      <c r="AP62">
+        <v>383</v>
+      </c>
+      <c r="AQ62">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="63" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN63">
+        <v>23</v>
+      </c>
+      <c r="AP63">
+        <v>447</v>
+      </c>
+      <c r="AQ63">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="64" spans="29:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN64">
+        <v>24</v>
+      </c>
+      <c r="AP64">
+        <v>512</v>
+      </c>
+      <c r="AQ64">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="65" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN65">
+        <v>25</v>
+      </c>
+      <c r="AP65">
+        <v>575</v>
+      </c>
+      <c r="AQ65">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="66" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN66">
+        <v>26</v>
+      </c>
+      <c r="AP66">
+        <v>574</v>
+      </c>
+      <c r="AQ66">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="67" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN67">
+        <v>27</v>
+      </c>
+      <c r="AP67">
+        <v>704</v>
+      </c>
+      <c r="AQ67">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="68" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN68">
+        <v>28</v>
+      </c>
+      <c r="AP68">
+        <v>704</v>
+      </c>
+      <c r="AQ68">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="69" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN69">
+        <v>29</v>
+      </c>
+      <c r="AP69">
+        <v>383</v>
+      </c>
+      <c r="AQ69">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="70" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN70">
+        <v>30</v>
+      </c>
+      <c r="AP70">
+        <v>383</v>
+      </c>
+      <c r="AQ70">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="71" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN71">
+        <v>31</v>
+      </c>
+      <c r="AP71">
+        <v>511</v>
+      </c>
+      <c r="AQ71">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="72" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN72">
+        <v>32</v>
+      </c>
+      <c r="AP72">
+        <v>639</v>
+      </c>
+      <c r="AQ72">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="73" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN73">
+        <v>33</v>
+      </c>
+      <c r="AP73">
+        <v>639</v>
+      </c>
+      <c r="AQ73">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="74" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN74">
+        <v>34</v>
+      </c>
+      <c r="AP74">
+        <v>639</v>
+      </c>
+      <c r="AQ74">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="75" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN75">
+        <v>35</v>
+      </c>
+      <c r="AP75">
+        <v>575</v>
+      </c>
+      <c r="AQ75">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="76" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN76">
+        <v>36</v>
+      </c>
+      <c r="AP76">
+        <v>511</v>
+      </c>
+      <c r="AQ76">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="77" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN77">
+        <v>37</v>
+      </c>
+      <c r="AP77">
+        <v>319</v>
+      </c>
+      <c r="AQ77">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="78" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN78">
+        <v>38</v>
+      </c>
+      <c r="AP78">
+        <v>255</v>
+      </c>
+      <c r="AQ78">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="79" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN79">
+        <v>39</v>
+      </c>
+      <c r="AP79">
+        <v>191</v>
+      </c>
+      <c r="AQ79">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="80" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN80">
+        <v>40</v>
+      </c>
+      <c r="AP80">
+        <v>194</v>
+      </c>
+      <c r="AQ80">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="81" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN81">
+        <v>41</v>
+      </c>
+      <c r="AP81">
+        <v>255</v>
+      </c>
+      <c r="AQ81">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="82" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN82">
+        <v>42</v>
+      </c>
+      <c r="AP82">
+        <v>382</v>
+      </c>
+      <c r="AQ82">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="83" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN83">
+        <v>43</v>
+      </c>
+      <c r="AP83">
+        <v>443</v>
+      </c>
+      <c r="AQ83">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="84" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN84">
+        <v>44</v>
+      </c>
+      <c r="AP84">
+        <v>94</v>
+      </c>
+      <c r="AQ84">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="85" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN85">
+        <v>45</v>
+      </c>
+      <c r="AP85">
+        <v>157</v>
+      </c>
+      <c r="AQ85">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="86" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN86">
+        <v>46</v>
+      </c>
+      <c r="AP86">
+        <v>383</v>
+      </c>
+      <c r="AQ86">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="87" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN87">
+        <v>47</v>
+      </c>
+      <c r="AP87">
+        <v>447</v>
+      </c>
+      <c r="AQ87">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="88" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN88">
+        <v>48</v>
+      </c>
+      <c r="AP88">
+        <v>448</v>
+      </c>
+      <c r="AQ88">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="89" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN89">
+        <v>49</v>
+      </c>
+      <c r="AP89">
+        <v>448</v>
+      </c>
+      <c r="AQ89">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="90" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN90">
+        <v>50</v>
+      </c>
+      <c r="AP90">
+        <v>383</v>
+      </c>
+      <c r="AQ90">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="91" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN91">
+        <v>51</v>
+      </c>
+      <c r="AP91">
+        <v>319</v>
+      </c>
+      <c r="AQ91">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN92">
+        <v>52</v>
+      </c>
+      <c r="AP92">
+        <v>318</v>
+      </c>
+      <c r="AQ92">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="93" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN93">
+        <v>53</v>
+      </c>
+      <c r="AP93">
+        <v>383</v>
+      </c>
+      <c r="AQ93">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="94" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN94">
+        <v>54</v>
+      </c>
+      <c r="AP94">
+        <v>700</v>
+      </c>
+      <c r="AQ94">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="95" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN95">
+        <v>55</v>
+      </c>
+      <c r="AP95">
+        <v>768</v>
+      </c>
+      <c r="AQ95">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="96" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN96">
+        <v>56</v>
+      </c>
+      <c r="AP96">
+        <v>767</v>
+      </c>
+      <c r="AQ96">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="40:43" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN97">
+        <v>57</v>
+      </c>
+      <c r="AP97">
+        <v>703</v>
+      </c>
+      <c r="AQ97">
+        <v>256</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>